<commit_message>
Finish evaluation of URL info
</commit_message>
<xml_diff>
--- a/evaluation/metrics.xlsx
+++ b/evaluation/metrics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesco\PycharmProjects\AntiPhish-LLM\evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\PycharmProjects\AntiPhish-LLM\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98E2BE3-3759-4F5A-821A-7BFFDC045AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27251DF7-7625-4023-AF0A-2FBB657A05D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>precision</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Binary classification metrics (predicted classes)</t>
+  </si>
+  <si>
+    <t>FP URL_Q=100</t>
   </si>
 </sst>
 </file>
@@ -77,7 +80,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -156,23 +159,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -457,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -474,45 +473,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="5"/>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2">
@@ -524,7 +522,7 @@
       <c r="D3" s="2">
         <v>0.97611010127239595</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>0.97715988083416006</v>
       </c>
       <c r="F3" s="2">
@@ -538,7 +536,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2">
@@ -550,7 +548,7 @@
       <c r="D4" s="2">
         <v>0.94925000000000004</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>0.94667717362752801</v>
       </c>
       <c r="F4" s="2">
@@ -564,7 +562,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2">
@@ -576,7 +574,7 @@
       <c r="D5" s="2">
         <v>0.999</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>0.99900099900099903</v>
       </c>
       <c r="F5" s="2">
@@ -590,7 +588,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2">
@@ -602,7 +600,7 @@
       <c r="D6" s="2">
         <v>0.999</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>0.99900099900099903</v>
       </c>
       <c r="F6" s="2">
@@ -616,7 +614,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2">
@@ -628,7 +626,7 @@
       <c r="D7" s="2">
         <v>0.999</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>0.99900099900099903</v>
       </c>
       <c r="F7" s="2">
@@ -642,7 +640,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2">
@@ -654,7 +652,7 @@
       <c r="D8" s="2">
         <v>0.999</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>0.99900099900099903</v>
       </c>
       <c r="F8" s="2">
@@ -668,7 +666,30 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.473407056345445</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.44950000000000001</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.62021386685063795</v>
+      </c>
+      <c r="F9" s="2">
+        <v>15.229762067346901</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2.6838750000000001E-2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.54341919999999999</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>